<commit_message>
Adição de calculo de média de vendas
</commit_message>
<xml_diff>
--- a/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
+++ b/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D19221A8-B4F3-D846-BE64-262285298ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71092495d8de150c/Repositórios/CC/Python/Nova pasta/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AD84553A-5D73-4870-80BD-F5AEAEC40501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8579AB-DB7B-4EF2-8F54-D186A391FDFE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -668,7 +673,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -736,8 +741,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -747,14 +752,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -762,12 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -993,22 +989,24 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="58.12109375" customWidth="1"/>
-    <col min="2" max="2" width="19.95703125" customWidth="1"/>
-    <col min="3" max="3" width="14.0234375" customWidth="1"/>
-    <col min="4" max="4" width="14.5625" customWidth="1"/>
-    <col min="5" max="5" width="15.1015625" customWidth="1"/>
-    <col min="6" max="6" width="18.87890625" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.6953125" customWidth="1"/>
-    <col min="9" max="9" width="15.1015625" customWidth="1"/>
+    <col min="1" max="1" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="14.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1060,7 +1058,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="14.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1086,7 +1084,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="14.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1112,7 +1110,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="14.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="14.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1164,7 +1162,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="14.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1190,7 +1188,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="14.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1216,7 +1214,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="14.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1242,7 +1240,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="14.25">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1268,7 +1266,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="14.25">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1294,7 +1292,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="14.25">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1320,7 +1318,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="14.25">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1346,11 +1344,11 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="14.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1372,7 +1370,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="14.25">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1398,7 +1396,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="14.25">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -1424,8 +1422,8 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:8" ht="14.25">
+      <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1450,8 +1448,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:8" ht="14.25">
+      <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1476,8 +1474,8 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:8" ht="14.25">
+      <c r="A19" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1502,8 +1500,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:8" ht="14.25">
+      <c r="A20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1528,8 +1526,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:8" ht="14.25">
+      <c r="A21" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1554,11 +1552,11 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="14.25">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1580,8 +1578,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:8" ht="14.25">
+      <c r="A23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1606,7 +1604,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="14.25">
       <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
@@ -1632,7 +1630,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="14.25">
       <c r="A25" s="5" t="s">
         <v>59</v>
       </c>
@@ -1658,7 +1656,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="14.25">
       <c r="A26" s="5" t="s">
         <v>61</v>
       </c>
@@ -1684,7 +1682,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="14.25">
       <c r="A27" s="5" t="s">
         <v>64</v>
       </c>
@@ -1710,11 +1708,11 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="14.25">
       <c r="A28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1736,7 +1734,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="14.25">
       <c r="A29" s="5" t="s">
         <v>68</v>
       </c>
@@ -1762,7 +1760,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="14.25">
       <c r="A30" s="5" t="s">
         <v>70</v>
       </c>
@@ -1788,7 +1786,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="14.25">
       <c r="A31" s="5" t="s">
         <v>72</v>
       </c>
@@ -1814,7 +1812,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="14.25">
       <c r="A32" s="5" t="s">
         <v>75</v>
       </c>
@@ -1840,7 +1838,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="14.25">
       <c r="A33" s="5" t="s">
         <v>78</v>
       </c>
@@ -1856,17 +1854,17 @@
       <c r="E33" s="6">
         <v>45172</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="8">
         <v>448</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="8" t="s">
         <v>80</v>
       </c>
       <c r="H33" s="4">
         <v>1100</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="14.25">
       <c r="A34" s="5" t="s">
         <v>81</v>
       </c>
@@ -1892,7 +1890,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="14.25">
       <c r="A35" s="5" t="s">
         <v>83</v>
       </c>
@@ -1918,7 +1916,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="14.25">
       <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
@@ -1937,14 +1935,14 @@
       <c r="F36" s="5">
         <v>424</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="8" t="s">
         <v>86</v>
       </c>
       <c r="H36" s="4">
         <v>1200</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="14.25">
       <c r="A37" s="5" t="s">
         <v>87</v>
       </c>
@@ -1963,14 +1961,14 @@
       <c r="F37" s="5">
         <v>529</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
       <c r="H37" s="4">
         <v>1200</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="14.25">
       <c r="A38" s="5" t="s">
         <v>88</v>
       </c>
@@ -1989,14 +1987,14 @@
       <c r="F38" s="5">
         <v>288</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="8" t="s">
         <v>86</v>
       </c>
       <c r="H38" s="4">
         <v>1500</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" ht="14.25">
       <c r="A39" s="3" t="s">
         <v>89</v>
       </c>
@@ -2022,7 +2020,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" ht="14.25">
       <c r="A40" s="5" t="s">
         <v>92</v>
       </c>
@@ -2048,7 +2046,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" ht="14.25">
       <c r="A41" s="5" t="s">
         <v>93</v>
       </c>
@@ -2067,15 +2065,15 @@
       <c r="F41" s="5">
         <v>336</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="8" t="s">
         <v>95</v>
       </c>
       <c r="H41" s="4">
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:8" ht="14.25">
+      <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2100,8 +2098,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:8" ht="28.5">
+      <c r="A43" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2119,15 +2117,15 @@
       <c r="F43" s="5">
         <v>376</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H43" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A44" s="10" t="s">
+    <row r="44" spans="1:8" ht="14.25">
+      <c r="A44" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2152,11 +2150,11 @@
         <v>960</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" ht="14.25">
       <c r="A45" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2178,7 +2176,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="26.25" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" ht="28.5">
       <c r="A46" s="5" t="s">
         <v>108</v>
       </c>
@@ -2197,14 +2195,14 @@
       <c r="F46" s="5">
         <v>240</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="8" t="s">
         <v>110</v>
       </c>
       <c r="H46" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" ht="14.25">
       <c r="A47" s="5" t="s">
         <v>111</v>
       </c>
@@ -2223,14 +2221,14 @@
       <c r="F47" s="5">
         <v>108</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="8" t="s">
         <v>113</v>
       </c>
       <c r="H47" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" ht="14.25">
       <c r="A48" s="5" t="s">
         <v>114</v>
       </c>
@@ -2249,14 +2247,14 @@
       <c r="F48" s="5">
         <v>112</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G48" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H48" s="4">
         <v>600</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:8" ht="14.25">
       <c r="A49" s="5" t="s">
         <v>117</v>
       </c>
@@ -2282,7 +2280,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:8" ht="14.25">
       <c r="A50" s="5" t="s">
         <v>120</v>
       </c>
@@ -2301,14 +2299,14 @@
       <c r="F50" s="5">
         <v>224</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="8" t="s">
         <v>122</v>
       </c>
       <c r="H50" s="4">
         <v>1200</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:8" ht="14.25">
       <c r="A51" s="3" t="s">
         <v>123</v>
       </c>
@@ -2327,14 +2325,14 @@
       <c r="F51" s="5">
         <v>400</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H51" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" ht="14.25">
       <c r="A52" s="3" t="s">
         <v>126</v>
       </c>
@@ -2353,14 +2351,14 @@
       <c r="F52" s="5">
         <v>240</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="4">
         <v>980</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:8" ht="14.25">
       <c r="A53" s="3" t="s">
         <v>127</v>
       </c>
@@ -2386,7 +2384,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:8" ht="14.25">
       <c r="A54" s="3" t="s">
         <v>130</v>
       </c>
@@ -2412,8 +2410,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A55" s="8" t="s">
+    <row r="55" spans="1:8" ht="14.25">
+      <c r="A55" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -2438,8 +2436,8 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:8" ht="28.5">
+      <c r="A56" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2457,15 +2455,15 @@
       <c r="F56" s="5">
         <v>280</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H56" s="4">
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:8" ht="14.25">
+      <c r="A57" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -2490,7 +2488,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" ht="14.25">
       <c r="A58" s="3" t="s">
         <v>135</v>
       </c>
@@ -2516,7 +2514,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" ht="28.5">
       <c r="A59" s="3" t="s">
         <v>136</v>
       </c>
@@ -2535,14 +2533,14 @@
       <c r="F59" s="5">
         <v>368</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="G59" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H59" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:8" ht="14.25">
       <c r="A60" s="3" t="s">
         <v>137</v>
       </c>
@@ -2568,7 +2566,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:8" ht="14.25">
       <c r="A61" s="3" t="s">
         <v>139</v>
       </c>
@@ -2594,7 +2592,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" ht="14.25">
       <c r="A62" s="5" t="s">
         <v>140</v>
       </c>
@@ -2620,7 +2618,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:8" ht="28.5">
       <c r="A63" s="5" t="s">
         <v>142</v>
       </c>
@@ -2639,14 +2637,14 @@
       <c r="F63" s="5">
         <v>488</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="8" t="s">
         <v>102</v>
       </c>
       <c r="H63" s="4">
         <v>670</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:8" ht="14.25">
       <c r="A64" s="5" t="s">
         <v>144</v>
       </c>
@@ -2672,7 +2670,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" ht="14.25">
       <c r="A65" s="5" t="s">
         <v>146</v>
       </c>
@@ -2691,14 +2689,14 @@
       <c r="F65" s="5">
         <v>630</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="G65" s="8" t="s">
         <v>148</v>
       </c>
       <c r="H65" s="4">
         <v>990</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" ht="14.25">
       <c r="A66" s="5" t="s">
         <v>149</v>
       </c>
@@ -2717,14 +2715,14 @@
       <c r="F66" s="5">
         <v>432</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="G66" s="8" t="s">
         <v>95</v>
       </c>
       <c r="H66" s="4">
         <v>900</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" ht="14.25">
       <c r="A67" s="5" t="s">
         <v>151</v>
       </c>
@@ -2750,7 +2748,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" ht="14.25">
       <c r="A68" s="5" t="s">
         <v>152</v>
       </c>
@@ -2776,7 +2774,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:8" ht="14.25">
       <c r="A69" s="3" t="s">
         <v>154</v>
       </c>
@@ -2802,7 +2800,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:8" ht="14.25">
       <c r="A70" s="5" t="s">
         <v>155</v>
       </c>
@@ -2828,7 +2826,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" ht="14.25">
       <c r="A71" s="3" t="s">
         <v>156</v>
       </c>
@@ -2854,7 +2852,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" ht="14.25">
       <c r="A72" s="3" t="s">
         <v>159</v>
       </c>
@@ -2873,14 +2871,14 @@
       <c r="F72" s="5">
         <v>392</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="G72" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H72" s="4">
         <v>1800</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:8" ht="14.25">
       <c r="A73" s="5" t="s">
         <v>160</v>
       </c>
@@ -2906,7 +2904,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:8" ht="14.25">
       <c r="A74" s="5" t="s">
         <v>161</v>
       </c>
@@ -2932,7 +2930,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:8" ht="14.25">
       <c r="A75" s="3" t="s">
         <v>162</v>
       </c>
@@ -2951,14 +2949,14 @@
       <c r="F75" s="5">
         <v>184</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G75" s="8" t="s">
         <v>163</v>
       </c>
       <c r="H75" s="4">
         <v>1570</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:8" ht="14.25">
       <c r="A76" s="3" t="s">
         <v>164</v>
       </c>
@@ -2984,7 +2982,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:8" ht="14.25">
       <c r="A77" s="3" t="s">
         <v>166</v>
       </c>
@@ -3010,7 +3008,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" ht="14.25">
       <c r="A78" s="3" t="s">
         <v>167</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" ht="14.25">
       <c r="A79" s="3" t="s">
         <v>168</v>
       </c>
@@ -3062,7 +3060,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:8" ht="14.25">
       <c r="A80" s="3" t="s">
         <v>170</v>
       </c>
@@ -3088,7 +3086,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" ht="14.25">
       <c r="A81" s="3" t="s">
         <v>172</v>
       </c>
@@ -3114,8 +3112,8 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A82" s="7" t="s">
+    <row r="82" spans="1:8" ht="14.25">
+      <c r="A82" s="5" t="s">
         <v>174</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -3140,7 +3138,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" ht="14.25">
       <c r="A83" s="3" t="s">
         <v>175</v>
       </c>
@@ -3166,7 +3164,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" ht="14.25">
       <c r="A84" s="3" t="s">
         <v>176</v>
       </c>
@@ -3192,7 +3190,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" ht="14.25">
       <c r="A85" s="3" t="s">
         <v>177</v>
       </c>
@@ -3218,7 +3216,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:8" ht="14.25">
       <c r="A86" s="3" t="s">
         <v>178</v>
       </c>
@@ -3237,15 +3235,15 @@
       <c r="F86" s="5">
         <v>288</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="G86" s="8" t="s">
         <v>180</v>
       </c>
       <c r="H86" s="4">
         <v>1600</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A87" s="7" t="s">
+    <row r="87" spans="1:8" ht="14.25">
+      <c r="A87" s="5" t="s">
         <v>181</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -3270,8 +3268,8 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A88" s="7" t="s">
+    <row r="88" spans="1:8" ht="14.25">
+      <c r="A88" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -3296,8 +3294,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A89" s="11" t="s">
+    <row r="89" spans="1:8" ht="14.25">
+      <c r="A89" s="5" t="s">
         <v>185</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -3322,7 +3320,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" ht="14.25">
       <c r="A90" s="3" t="s">
         <v>186</v>
       </c>
@@ -3348,7 +3346,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:8" ht="14.25">
       <c r="A91" s="3" t="s">
         <v>187</v>
       </c>
@@ -3374,8 +3372,8 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A92" s="7" t="s">
+    <row r="92" spans="1:8" ht="14.25">
+      <c r="A92" s="5" t="s">
         <v>188</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -3400,8 +3398,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A93" s="8" t="s">
+    <row r="93" spans="1:8" ht="14.25">
+      <c r="A93" s="7" t="s">
         <v>190</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -3426,8 +3424,8 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A94" s="8" t="s">
+    <row r="94" spans="1:8" ht="14.25">
+      <c r="A94" s="7" t="s">
         <v>192</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -3452,8 +3450,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A95" s="8" t="s">
+    <row r="95" spans="1:8" ht="14.25">
+      <c r="A95" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -3478,8 +3476,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A96" s="8" t="s">
+    <row r="96" spans="1:8" ht="14.25">
+      <c r="A96" s="7" t="s">
         <v>197</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -3504,8 +3502,8 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A97" s="8" t="s">
+    <row r="97" spans="1:8" ht="14.25">
+      <c r="A97" s="7" t="s">
         <v>198</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -3523,15 +3521,15 @@
       <c r="F97" s="5">
         <v>336</v>
       </c>
-      <c r="G97" s="9" t="s">
+      <c r="G97" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H97" s="4">
         <v>1150</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A98" s="8" t="s">
+    <row r="98" spans="1:8" ht="14.25">
+      <c r="A98" s="7" t="s">
         <v>200</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -3549,15 +3547,15 @@
       <c r="F98" s="5">
         <v>342</v>
       </c>
-      <c r="G98" s="9" t="s">
+      <c r="G98" s="8" t="s">
         <v>202</v>
       </c>
       <c r="H98" s="4">
         <v>1300</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A99" s="8" t="s">
+    <row r="99" spans="1:8" ht="14.25">
+      <c r="A99" s="7" t="s">
         <v>203</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -3582,8 +3580,8 @@
         <v>950</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A100" s="8" t="s">
+    <row r="100" spans="1:8" ht="14.25">
+      <c r="A100" s="7" t="s">
         <v>206</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -3608,8 +3606,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A101" s="8" t="s">
+    <row r="101" spans="1:8" ht="14.25">
+      <c r="A101" s="7" t="s">
         <v>208</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -3627,18 +3625,19 @@
       <c r="F101" s="5">
         <v>656</v>
       </c>
-      <c r="G101" s="9" t="s">
+      <c r="G101" s="8" t="s">
         <v>95</v>
       </c>
       <c r="H101" s="4">
         <v>980</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="12.75" x14ac:dyDescent="0.15">
-      <c r="A102" s="12"/>
-      <c r="G102" s="13"/>
+    <row r="102" spans="1:8" ht="14.25">
+      <c r="A102" s="9"/>
+      <c r="G102" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Impressão de média e cálculo de gênero mais vendido
</commit_message>
<xml_diff>
--- a/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
+++ b/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71092495d8de150c/Repositórios/CC/Python/Nova pasta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71092495d8de150c/Repositórios/CC/Python/Análise de dados com pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AD84553A-5D73-4870-80BD-F5AEAEC40501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8579AB-DB7B-4EF2-8F54-D186A391FDFE}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -784,6 +784,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -989,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Reorganização de vendas por gênero
</commit_message>
<xml_diff>
--- a/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
+++ b/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
@@ -993,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Cálculo de editora que mais vendeu
</commit_message>
<xml_diff>
--- a/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
+++ b/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71092495d8de150c/Repositórios/CC/Python/Análise de dados com pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AD84553A-5D73-4870-80BD-F5AEAEC40501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8579AB-DB7B-4EF2-8F54-D186A391FDFE}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{AD84553A-5D73-4870-80BD-F5AEAEC40501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC80D44D-76D8-45EE-A1A7-B6A6784BA4DE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -993,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -2957,7 +2957,7 @@
         <v>163</v>
       </c>
       <c r="H75" s="4">
-        <v>1570</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="14.25">

</xml_diff>

<commit_message>
Cálculo de autor que mais vendeu + resultado debug
</commit_message>
<xml_diff>
--- a/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
+++ b/Vendas rede de livrarias(os 100 titulos mais vendidos).xlsx
@@ -993,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>